<commit_message>
Latest Updates from Costco
</commit_message>
<xml_diff>
--- a/Costco/CostcoHomePage.xlsx
+++ b/Costco/CostcoHomePage.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3160" yWindow="600" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="6520" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Aboutus" sheetId="1" r:id="rId1"/>
+    <sheet name="AboutUs" sheetId="1" r:id="rId1"/>
     <sheet name="Membership" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -20,57 +20,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>Charitable Contributions</t>
+  </si>
+  <si>
+    <t>Company Information</t>
+  </si>
+  <si>
+    <t>Sustainability Commitment</t>
+  </si>
+  <si>
+    <t>Investor Relations</t>
+  </si>
+  <si>
+    <t>Jobs</t>
+  </si>
+  <si>
+    <t>Logo and Media Requests</t>
+  </si>
+  <si>
+    <t>Product Videos</t>
+  </si>
+  <si>
+    <t>The Costco Connection</t>
+  </si>
+  <si>
+    <t>Employee Site</t>
+  </si>
+  <si>
+    <t>Membership</t>
+  </si>
+  <si>
+    <t>Join Now</t>
+  </si>
+  <si>
+    <t>Member Privileges</t>
+  </si>
+  <si>
+    <t>Executive Membership Terms</t>
+  </si>
+  <si>
+    <t>Sign In or Register</t>
+  </si>
+  <si>
+    <t>Credit Card</t>
+  </si>
+  <si>
+    <t>Kirkland Signature</t>
+  </si>
   <si>
     <t>About Us</t>
   </si>
   <si>
-    <t>Charitable Contributions</t>
-  </si>
-  <si>
-    <t>Company Information</t>
-  </si>
-  <si>
-    <t>Sustainability Commitment</t>
-  </si>
-  <si>
-    <t>Investor Relations</t>
-  </si>
-  <si>
-    <t>Jobs</t>
-  </si>
-  <si>
-    <t>Logo and Media Requests</t>
-  </si>
-  <si>
-    <t>Product Videos</t>
-  </si>
-  <si>
-    <t>The Costco Connection</t>
-  </si>
-  <si>
-    <t>Quick and Easy Recipe Videos</t>
-  </si>
-  <si>
-    <t>Employee Site</t>
-  </si>
-  <si>
-    <t>Membership</t>
-  </si>
-  <si>
-    <t>Join Now</t>
-  </si>
-  <si>
-    <t>Member Privileges</t>
-  </si>
-  <si>
-    <t>Executive Membership Terms</t>
-  </si>
-  <si>
-    <t>Sign In or Register</t>
-  </si>
-  <si>
-    <t>Credit Card</t>
+    <t>Quick &amp; Easy Recipe Videos</t>
   </si>
 </sst>
 </file>
@@ -132,8 +135,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -142,9 +147,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -474,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -488,57 +495,62 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -567,32 +579,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>